<commit_message>
Altered to get mean of columns C and D from 3D Cell bodies tab
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -46,8 +46,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,57 +422,298 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="52" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" style="1" min="5" max="5"/>
+    <col width="20" customWidth="1" style="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="20" customWidth="1" min="18" max="18"/>
+    <col width="20" customWidth="1" min="19" max="19"/>
+    <col width="20" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="21" max="21"/>
+    <col width="20" customWidth="1" min="22" max="22"/>
+    <col width="20" customWidth="1" min="23" max="23"/>
+    <col width="20" customWidth="1" min="24" max="24"/>
+    <col width="20" customWidth="1" min="25" max="25"/>
+    <col width="20" customWidth="1" min="26" max="26"/>
+    <col width="20" customWidth="1" min="27" max="27"/>
+    <col width="20" customWidth="1" min="28" max="28"/>
+    <col width="20" customWidth="1" min="29" max="29"/>
+    <col width="20" customWidth="1" min="30" max="30"/>
+    <col width="20" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Data File</t>
-        </is>
-      </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Total Markers Counted</t>
+          <t>Perimeter(µm)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Number of Sections</t>
+          <t>Area(µm²)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>User Defined Mounted Thickness</t>
+          <t>Feret Max(µm)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Estimated Population using User Defined Section Thickness</t>
+          <t>Enclosed Volume(µm³)</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Surface Area(µm²)</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>n of 3D</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Cell Body Length(µm)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Cell Body Mean Length</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Cell Body Area (µm²)</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Cell Body Mean Area</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Cell Body Surface(µm²)</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Cell Body Mean Surface</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Cell Body Volume(µm³)</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Cell Body Mean Volume</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Axon Length(µm)</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Axon Mean Length</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Axon Area (µm²)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Axon Mean Area</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Axon Surface(µm²)</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Axon Mean Surface</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Axon Volume(µm³)</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Axon Mean Volume</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>Dendrite Length(µm)</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Dendrite Mean Length</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Dendrite Area (µm²)</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Dendrite Mean Area</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>Dendrite Surface(µm²)</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>Dendrite Mean Surface</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>Dendrite Volume(µm³)</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Dendrite Mean Volume</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5HTR1a P5 CTR8 lumbar</t>
+          <t>05042016 in1 08232019 gfp reconstruction</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>254</v>
+        <v>130.19</v>
       </c>
       <c r="C2" t="n">
-        <v>17</v>
+        <v>465.7</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>35.25</v>
       </c>
       <c r="E2" t="n">
-        <v>3484.88</v>
+        <v>1063.275887096774</v>
+      </c>
+      <c r="F2" t="n">
+        <v>524.4065322580645</v>
+      </c>
+      <c r="G2" t="n">
+        <v>124</v>
+      </c>
+      <c r="H2" t="n">
+        <v>36868.3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>38.97</v>
+      </c>
+      <c r="J2" t="n">
+        <v>96640.7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>102.16</v>
+      </c>
+      <c r="L2" t="n">
+        <v>69178.3</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>3276.01</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>